<commit_message>
Refactored Logger and added unit tests.
</commit_message>
<xml_diff>
--- a/rules/CommandMap.xlsx
+++ b/rules/CommandMap.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45080" yWindow="460" windowWidth="20640" windowHeight="21060" tabRatio="500"/>
+    <workbookView xWindow="39960" yWindow="460" windowWidth="38560" windowHeight="28260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Command Map" sheetId="1" r:id="rId1"/>
     <sheet name="Ref" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Command Map'!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Command Map'!$G$2:$G$25</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="96">
   <si>
     <t>ID</t>
   </si>
@@ -220,6 +221,102 @@
   </si>
   <si>
     <t>Removes an association between two elements.</t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>CreateElement</t>
+  </si>
+  <si>
+    <t>CreateElementDefinition</t>
+  </si>
+  <si>
+    <t>DeleteAssociation</t>
+  </si>
+  <si>
+    <t>DeleteElementDefintion</t>
+  </si>
+  <si>
+    <t>EditAssociation</t>
+  </si>
+  <si>
+    <t>EditDataSet</t>
+  </si>
+  <si>
+    <t>EditElement</t>
+  </si>
+  <si>
+    <t>EditElementDefintion</t>
+  </si>
+  <si>
+    <t>EditElementPropertyDefinition</t>
+  </si>
+  <si>
+    <t>EngineCommands</t>
+  </si>
+  <si>
+    <t>FindAssociationById</t>
+  </si>
+  <si>
+    <t>FindDataSetById</t>
+  </si>
+  <si>
+    <t>FindDataSetByName</t>
+  </si>
+  <si>
+    <t>FindDownStreamElementsByElementId</t>
+  </si>
+  <si>
+    <t>FindElementById</t>
+  </si>
+  <si>
+    <t>FindElementDefinition</t>
+  </si>
+  <si>
+    <t>FindElementDefinitionById</t>
+  </si>
+  <si>
+    <t>FindElementDefinitionByName</t>
+  </si>
+  <si>
+    <t>FindInboundAssociationsByElementId</t>
+  </si>
+  <si>
+    <t>FindOutboundAssociationsByElementId</t>
+  </si>
+  <si>
+    <t>FindUpStreamElementsByElementId</t>
+  </si>
+  <si>
+    <t>ListAllElementDefinitions</t>
+  </si>
+  <si>
+    <t>RemoveAssociationField</t>
+  </si>
+  <si>
+    <t>RemoveElementField</t>
+  </si>
+  <si>
+    <t>RemoveElementPropertyDefinition</t>
+  </si>
+  <si>
+    <t>RemoveInboundAssociations</t>
+  </si>
+  <si>
+    <t>RemoveOutboundAssociations</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Planned</t>
+  </si>
+  <si>
+    <t>Blocked</t>
   </si>
 </sst>
 </file>
@@ -263,7 +360,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -272,11 +369,590 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="7" tint="-0.499984740745262"/>
@@ -649,10 +1325,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,9 +1338,11 @@
     <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="32" customWidth="1"/>
     <col min="6" max="6" width="38.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="52.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,8 +1361,11 @@
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -703,8 +1384,14 @@
       <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -724,8 +1411,14 @@
       <c r="F3" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>3</v>
@@ -745,8 +1438,14 @@
       <c r="F4" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -766,8 +1465,14 @@
       <c r="F5" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -787,8 +1492,14 @@
       <c r="F6" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -808,8 +1519,14 @@
       <c r="F7" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -829,8 +1546,14 @@
       <c r="F8" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -850,8 +1573,14 @@
       <c r="F9" s="3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -871,8 +1600,14 @@
       <c r="F10" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
+        <v>94</v>
+      </c>
+      <c r="H10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -892,8 +1627,14 @@
       <c r="F11" s="3" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -913,8 +1654,14 @@
       <c r="F12" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -934,8 +1681,14 @@
       <c r="F13" s="3" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -955,8 +1708,14 @@
       <c r="F14" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -976,8 +1735,14 @@
       <c r="F15" s="3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -997,8 +1762,14 @@
       <c r="F16" s="3" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="G16" t="s">
+        <v>94</v>
+      </c>
+      <c r="H16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1018,8 +1789,14 @@
       <c r="F17" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" ht="80" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>94</v>
+      </c>
+      <c r="H17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>A17+1</f>
         <v>17</v>
@@ -1039,8 +1816,14 @@
       <c r="F18" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" ref="A19:A23" si="1">A18+1</f>
         <v>18</v>
@@ -1060,8 +1843,14 @@
       <c r="F19" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1081,8 +1870,14 @@
       <c r="F20" s="3" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+      <c r="H20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1102,8 +1897,14 @@
       <c r="F21" s="3" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>94</v>
+      </c>
+      <c r="H21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1123,8 +1924,14 @@
       <c r="F22" s="3" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="G22" t="s">
+        <v>94</v>
+      </c>
+      <c r="H22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1144,8 +1951,14 @@
       <c r="F23" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" t="s">
+        <v>94</v>
+      </c>
+      <c r="H23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1164,8 +1977,14 @@
       <c r="F24" s="3" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="G24" t="s">
+        <v>94</v>
+      </c>
+      <c r="H24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1184,27 +2003,67 @@
       <c r="F25" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="G25" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
-  <conditionalFormatting sqref="A1:F1048576">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="A1:G1048576 G1">
+    <cfRule type="expression" dxfId="7" priority="4" stopIfTrue="1">
+      <formula>$D1="ELEMENT_DEFINITION"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
       <formula>$D1="ASSOCIATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
       <formula>$D1="ELEMENT"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
+    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
       <formula>$D1="DATA_SET"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
-      <formula>$D1="ELEMENT_DEFINITION"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Ref!$A$1:$A$8</xm:f>
@@ -1229,6 +2088,12 @@
           </x14:formula1>
           <xm:sqref>D1:D1048576</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Ref!$I$2:$I$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G25</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -1240,10 +2105,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor rgb="FFC00000"/>
   </sheetPr>
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1255,9 +2120,10 @@
     <col min="5" max="5" width="19.6640625" customWidth="1"/>
     <col min="6" max="6" width="2" customWidth="1"/>
     <col min="7" max="7" width="31.33203125" customWidth="1"/>
+    <col min="8" max="8" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -1270,8 +2136,11 @@
       <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1284,8 +2153,11 @@
       <c r="G2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1298,8 +2170,11 @@
       <c r="G3" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1312,8 +2187,11 @@
       <c r="G4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1324,7 +2202,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1332,7 +2210,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1340,7 +2218,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1348,42 +2226,42 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G9" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G13" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G14" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="G16" t="s">
         <v>51</v>
       </c>
@@ -1416,6 +2294,184 @@
     <row r="22" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G22" t="s">
         <v>58</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A32"/>
+  <sheetViews>
+    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="37.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Continued to refine the protocol buffer definitions
Implemented basic 0MQ Actor. Note: Test failing due to timing issue.
</commit_message>
<xml_diff>
--- a/rules/CommandMap.xlsx
+++ b/rules/CommandMap.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="39960" yWindow="460" windowWidth="38560" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="27320" yWindow="460" windowWidth="51200" windowHeight="28340" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Command Map" sheetId="1" r:id="rId1"/>
     <sheet name="Ref" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Internal Cmds" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Command Map'!$G$2:$G$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Internal Cmds'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="115">
   <si>
     <t>ID</t>
   </si>
@@ -253,9 +254,6 @@
     <t>EditElementPropertyDefinition</t>
   </si>
   <si>
-    <t>EngineCommands</t>
-  </si>
-  <si>
     <t>FindAssociationById</t>
   </si>
   <si>
@@ -317,6 +315,84 @@
   </si>
   <si>
     <t>Blocked</t>
+  </si>
+  <si>
+    <t>Association ID</t>
+  </si>
+  <si>
+    <t>Dataset ID</t>
+  </si>
+  <si>
+    <t>Element ID</t>
+  </si>
+  <si>
+    <t>Element Definition ID</t>
+  </si>
+  <si>
+    <t>Association Object</t>
+  </si>
+  <si>
+    <t>Dataset Object</t>
+  </si>
+  <si>
+    <t>List[Element]</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>Element Definition</t>
+  </si>
+  <si>
+    <t>List[Association]</t>
+  </si>
+  <si>
+    <t>List[ElementDefinition]</t>
+  </si>
+  <si>
+    <t>List[DataSet]</t>
+  </si>
+  <si>
+    <t>Nothing (Unit)</t>
+  </si>
+  <si>
+    <t>Command Return Type</t>
+  </si>
+  <si>
+    <t>Engine Return Type</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>ID: String
+associationType: String
+fields: Map[String, Any]
+startingElementId: String
+endingElementId: String
+creationgType:String
+lastModifiedType: String</t>
+  </si>
+  <si>
+    <t>id: String
+name: String
+description: String
+creationTime: String
+lastModifiedTime: String</t>
+  </si>
+  <si>
+    <t>id: String
+elementType: String
+elementDescription: String
+fields: Map[String, Any]
+creationTime: String
+lastModifiedTime: String</t>
+  </si>
+  <si>
+    <t>id: String
+name: String
+description: String
+properties:List[PropertyDefinition]</t>
   </si>
 </sst>
 </file>
@@ -379,6 +455,54 @@
   <dxfs count="28">
     <dxf>
       <font>
+        <color theme="7" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="4" tint="-0.499984740745262"/>
       </font>
       <fill>
@@ -427,78 +551,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="4" tint="-0.499984740745262"/>
       </font>
       <fill>
@@ -552,6 +604,30 @@
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
       <border>
@@ -1325,10 +1401,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:H32"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1362,7 +1438,7 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -1385,7 +1461,7 @@
         <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H2" t="s">
         <v>33</v>
@@ -1412,7 +1488,7 @@
         <v>35</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H3" t="s">
         <v>21</v>
@@ -1439,7 +1515,7 @@
         <v>39</v>
       </c>
       <c r="G4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H4" t="s">
         <v>65</v>
@@ -1466,7 +1542,7 @@
         <v>38</v>
       </c>
       <c r="G5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H5" t="s">
         <v>66</v>
@@ -1493,7 +1569,7 @@
         <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H6" t="s">
         <v>67</v>
@@ -1520,7 +1596,7 @@
         <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H7" t="s">
         <v>27</v>
@@ -1547,7 +1623,7 @@
         <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H8" t="s">
         <v>68</v>
@@ -1574,7 +1650,7 @@
         <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H9" t="s">
         <v>69</v>
@@ -1601,7 +1677,7 @@
         <v>44</v>
       </c>
       <c r="G10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H10" t="s">
         <v>70</v>
@@ -1628,7 +1704,7 @@
         <v>45</v>
       </c>
       <c r="G11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H11" t="s">
         <v>71</v>
@@ -1655,7 +1731,7 @@
         <v>46</v>
       </c>
       <c r="G12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H12" t="s">
         <v>72</v>
@@ -1682,7 +1758,7 @@
         <v>47</v>
       </c>
       <c r="G13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H13" t="s">
         <v>73</v>
@@ -1709,7 +1785,7 @@
         <v>48</v>
       </c>
       <c r="G14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H14" t="s">
         <v>74</v>
@@ -1736,7 +1812,7 @@
         <v>49</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H15" t="s">
         <v>75</v>
@@ -1763,7 +1839,7 @@
         <v>52</v>
       </c>
       <c r="G16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H16" t="s">
         <v>76</v>
@@ -1790,7 +1866,7 @@
         <v>53</v>
       </c>
       <c r="G17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H17" t="s">
         <v>77</v>
@@ -1817,7 +1893,7 @@
         <v>54</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H18" t="s">
         <v>78</v>
@@ -1844,7 +1920,7 @@
         <v>55</v>
       </c>
       <c r="G19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H19" t="s">
         <v>79</v>
@@ -1871,7 +1947,7 @@
         <v>56</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H20" t="s">
         <v>80</v>
@@ -1898,7 +1974,7 @@
         <v>57</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H21" t="s">
         <v>81</v>
@@ -1925,7 +2001,7 @@
         <v>61</v>
       </c>
       <c r="G22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H22" t="s">
         <v>82</v>
@@ -1952,7 +2028,7 @@
         <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H23" t="s">
         <v>83</v>
@@ -1978,7 +2054,7 @@
         <v>62</v>
       </c>
       <c r="G24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H24" t="s">
         <v>84</v>
@@ -2004,7 +2080,7 @@
         <v>63</v>
       </c>
       <c r="G25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H25" t="s">
         <v>85</v>
@@ -2012,12 +2088,12 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
-        <v>86</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H27" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
@@ -2040,24 +2116,19 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H32" t="s">
-        <v>91</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:G1048576 G1">
-    <cfRule type="expression" dxfId="7" priority="4" stopIfTrue="1">
-      <formula>$D1="ELEMENT_DEFINITION"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="1" stopIfTrue="1">
+  <conditionalFormatting sqref="A1:G1048576">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>$D1="ASSOCIATION"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
       <formula>$D1="ELEMENT"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
       <formula>$D1="DATA_SET"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+      <formula>$D1="ELEMENT_DEFINITION"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2137,7 +2208,7 @@
         <v>19</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2154,7 +2225,7 @@
         <v>29</v>
       </c>
       <c r="I2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -2171,7 +2242,7 @@
         <v>30</v>
       </c>
       <c r="I3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -2188,7 +2259,7 @@
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -2303,178 +2374,355 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A32"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39" style="3" customWidth="1"/>
+    <col min="5" max="5" width="41.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="112" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>99</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B7" t="s">
+        <v>96</v>
+      </c>
+      <c r="C7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="80" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>76</v>
+      </c>
+      <c r="B10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="96" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B17" t="s">
+        <v>98</v>
+      </c>
+      <c r="C17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>73</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>88</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="B20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="B22" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="B27" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="B28" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>91</v>
+      <c r="B31" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1">
+    <sortState ref="A2:D31">
+      <sortCondition ref="B1:B31"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added first draft of very basic decision tree.
</commit_message>
<xml_diff>
--- a/rules/CommandMap.xlsx
+++ b/rules/CommandMap.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27320" yWindow="460" windowWidth="51200" windowHeight="28340" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Command Map" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="Internal Cmds" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Command Map'!$G$2:$G$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Command Map'!$A$1:$H$31</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Internal Cmds'!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -452,583 +452,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="7" tint="-0.499984740745262"/>
@@ -1398,13 +822,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1441,7 +865,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1467,7 +891,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1494,7 +918,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>3</v>
@@ -1521,7 +945,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1656,7 +1080,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1683,7 +1107,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1710,7 +1134,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1737,7 +1161,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1872,7 +1296,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>A17+1</f>
         <v>17</v>
@@ -1899,7 +1323,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" ref="A19:A23" si="1">A18+1</f>
         <v>18</v>
@@ -1926,7 +1350,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1953,7 +1377,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1980,7 +1404,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -2007,7 +1431,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -2034,7 +1458,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2060,7 +1484,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2086,37 +1510,44 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="H27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H31">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="USER_SPACE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="A1:G1048576">
     <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>$D1="ASSOCIATION"</formula>
@@ -2376,7 +1807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added basic construction of Decision Tree from JSON Rules directory.
</commit_message>
<xml_diff>
--- a/rules/CommandMap.xlsx
+++ b/rules/CommandMap.xlsx
@@ -822,13 +822,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0">
+  <sheetPr enableFormatConditionsCalculation="0">
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -865,7 +865,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -891,7 +891,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -918,7 +918,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>3</v>
@@ -945,7 +945,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1080,7 +1080,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1107,7 +1107,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1134,7 +1134,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1161,7 +1161,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1296,7 +1296,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="80" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" ht="80" x14ac:dyDescent="0.2">
       <c r="A18">
         <f>A17+1</f>
         <v>17</v>
@@ -1323,7 +1323,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" ref="A19:A23" si="1">A18+1</f>
         <v>18</v>
@@ -1350,7 +1350,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="1"/>
         <v>19</v>
@@ -1377,7 +1377,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="1"/>
         <v>20</v>
@@ -1404,7 +1404,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="1"/>
         <v>21</v>
@@ -1431,7 +1431,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="1"/>
         <v>22</v>
@@ -1458,7 +1458,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1510,44 +1510,38 @@
         <v>85</v>
       </c>
     </row>
-    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H26" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H27" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H28" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H29" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H30" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H31" t="s">
         <v>90</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H31">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="USER_SPACE"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:H31"/>
   <conditionalFormatting sqref="A1:G1048576">
     <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
       <formula>$D1="ASSOCIATION"</formula>

</xml_diff>